<commit_message>
Update Santo amaro indices pluviométricos.xlsx
</commit_message>
<xml_diff>
--- a/Santo amaro indices pluviométricos.xlsx
+++ b/Santo amaro indices pluviométricos.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/65506b31b36bc35e/Área de Trabalho/UNIP/TCC/TCC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="118" documentId="13_ncr:1_{7A022D26-E242-4E02-8392-C8A4A1725365}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A019AE82-F268-4145-9E3C-868D4C2CE624}"/>
+  <xr:revisionPtr revIDLastSave="119" documentId="13_ncr:1_{7A022D26-E242-4E02-8392-C8A4A1725365}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{47727C62-86BF-4DB1-879A-177470A26ED0}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{02732F80-8D48-4307-8EAB-238FF97CB285}"/>
   </bookViews>
@@ -1004,14 +1004,15 @@
   <dimension ref="A1:P29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="Q18" sqref="Q18"/>
+      <selection activeCell="O31" sqref="O31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="19.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="34" bestFit="1" customWidth="1"/>
-    <col min="4" max="13" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="12" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21.7109375" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="9.28515625" customWidth="1"/>
     <col min="16" max="16" width="21.7109375" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="19.7109375" bestFit="1" customWidth="1"/>

</xml_diff>